<commit_message>
67: Debug some issue about ASC function. Named V0.22.
</commit_message>
<xml_diff>
--- a/Objects/PGS7-0-22_20250326-BurnFile/PGS7000_Modbus寄存器和Elmos寄存器和CM参数关系.xlsx
+++ b/Objects/PGS7-0-22_20250326-BurnFile/PGS7000_Modbus寄存器和Elmos寄存器和CM参数关系.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="425">
   <si>
     <t>Modbus Register Address and E703 Register Address Map</t>
   </si>
@@ -1760,6 +1760,21 @@
   </si>
   <si>
     <t>ASC_Adjust_Value3:ASCde校准值。</t>
+  </si>
+  <si>
+    <t>0x036A</t>
+  </si>
+  <si>
+    <t>ASC_Tmpr_Rate：温度变化率实时值。单位0.1℃/Min</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>0x036B</t>
+  </si>
+  <si>
+    <t>ASC_Humi_Rate：湿度变化率实时值。单位0.1%/Min</t>
   </si>
 </sst>
 </file>
@@ -6674,10 +6689,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D109"/>
+  <dimension ref="A1:D111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C111" sqref="C111"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="C115" sqref="C115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
@@ -7935,6 +7950,34 @@
       </c>
       <c r="D109" t="s">
         <v>413</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" s="11" t="s">
+        <v>420</v>
+      </c>
+      <c r="B110" s="11">
+        <v>874</v>
+      </c>
+      <c r="C110" s="19" t="s">
+        <v>421</v>
+      </c>
+      <c r="D110" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" s="11" t="s">
+        <v>423</v>
+      </c>
+      <c r="B111" s="11">
+        <v>875</v>
+      </c>
+      <c r="C111" s="19" t="s">
+        <v>424</v>
+      </c>
+      <c r="D111" t="s">
+        <v>422</v>
       </c>
     </row>
   </sheetData>

</xml_diff>